<commit_message>
Began adding labels for rooms on board
</commit_message>
<xml_diff>
--- a/testScenarios.xlsx
+++ b/testScenarios.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24240" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -99,9 +100,6 @@
     <t>Pool</t>
   </si>
   <si>
-    <t>Bowling Alley</t>
-  </si>
-  <si>
     <t>Study</t>
   </si>
   <si>
@@ -136,6 +134,9 @@
   </si>
   <si>
     <t>Target Test scenarios</t>
+  </si>
+  <si>
+    <t>Bar</t>
   </si>
 </sst>
 </file>
@@ -398,6 +399,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -445,7 +449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,7 +484,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -692,7 +696,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,10 +794,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>2</v>
@@ -805,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>4</v>
@@ -817,10 +821,10 @@
         <v>4</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>6</v>
@@ -853,10 +857,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>2</v>
@@ -868,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>4</v>
@@ -880,10 +884,10 @@
         <v>4</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>6</v>
@@ -917,10 +921,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>2</v>
@@ -932,7 +936,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>4</v>
@@ -944,13 +948,13 @@
         <v>4</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>6</v>
@@ -975,52 +979,52 @@
         <v>3</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R5" s="7" t="s">
         <v>7</v>
@@ -1045,58 +1049,58 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T6" s="11">
         <f t="shared" si="2"/>
@@ -1118,25 +1122,25 @@
         <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>20</v>
@@ -1145,28 +1149,28 @@
         <v>20</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T7" s="11">
         <f t="shared" si="2"/>
@@ -1197,16 +1201,16 @@
         <v>18</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>20</v>
@@ -1215,22 +1219,22 @@
         <v>20</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R8" s="6" t="s">
         <v>8</v>
@@ -1267,16 +1271,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>20</v>
@@ -1285,22 +1289,22 @@
         <v>20</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R9" s="6" t="s">
         <v>8</v>
@@ -1337,7 +1341,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>20</v>
@@ -1364,13 +1368,13 @@
         <v>20</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R10" s="18" t="s">
         <v>9</v>
@@ -1383,7 +1387,7 @@
         <v>8</v>
       </c>
       <c r="U10" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="V10" s="3" t="s">
         <v>8</v>
@@ -1407,7 +1411,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>20</v>
@@ -1434,13 +1438,13 @@
         <v>20</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>9</v>
@@ -1453,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="U11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V11" s="3" t="s">
         <v>10</v>
@@ -1477,16 +1481,16 @@
         <v>19</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>20</v>
@@ -1495,22 +1499,22 @@
         <v>20</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R12" s="6" t="s">
         <v>8</v>
@@ -1523,7 +1527,7 @@
         <v>10</v>
       </c>
       <c r="U12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V12" s="3" t="s">
         <v>12</v>
@@ -1547,16 +1551,16 @@
         <v>18</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>20</v>
@@ -1565,22 +1569,22 @@
         <v>20</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>8</v>
@@ -1593,7 +1597,7 @@
         <v>11</v>
       </c>
       <c r="U13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V13" s="3" t="s">
         <v>14</v>
@@ -1617,16 +1621,16 @@
         <v>18</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>20</v>
@@ -1635,35 +1639,35 @@
         <v>20</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T14" s="11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="U14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V14" s="5" t="s">
         <v>20</v>
@@ -1678,55 +1682,55 @@
         <v>16</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T15" s="11">
         <f t="shared" si="2"/>
@@ -1739,49 +1743,49 @@
         <v>14</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P16" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>11</v>
@@ -1803,49 +1807,49 @@
         <v>15</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P17" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>10</v>
@@ -1879,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>12</v>
@@ -1900,13 +1904,13 @@
         <v>12</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>10</v>
@@ -1943,10 +1947,10 @@
         <v>14</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>12</v>
@@ -1967,10 +1971,10 @@
         <v>12</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>10</v>
@@ -2007,10 +2011,10 @@
         <v>14</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>12</v>
@@ -2031,10 +2035,10 @@
         <v>12</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>10</v>
@@ -2128,13 +2132,13 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
@@ -2144,7 +2148,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C24" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -2153,7 +2157,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -2162,7 +2166,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
@@ -2171,7 +2175,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>

</xml_diff>